<commit_message>
added parametrisation with hashTable
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testingData.xlsx
+++ b/src/test/resources/excel/testingData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manish_Katepallewar\eclipse-workspace\TestNGLearning\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FB3971-7E3E-4CCE-876F-457F855FD072}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411D02FE-7906-4DB7-8063-10FA1C8830BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="915" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{F43DADB2-5907-433D-A30E-9CB925CA857A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Manish1</t>
-  </si>
-  <si>
     <t>PP</t>
   </si>
   <si>
@@ -58,6 +55,21 @@
   </si>
   <si>
     <t>is_correct</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>TTT</t>
   </si>
 </sst>
 </file>
@@ -409,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47641BF6-EE33-4D95-BFA9-E2CE9B3311AE}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,18 +433,24 @@
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -442,16 +460,28 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="D3">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>